<commit_message>
small changes in students files and presentation files
</commit_message>
<xml_diff>
--- a/docs/projects/excel/01/01.xlsx
+++ b/docs/projects/excel/01/01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jooan\Documents\GitHub Projects\digitalis_kultura\docs\projects\excel\01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACFA5BC-9D60-4031-9C72-224CC09FFB4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD9722C-AD76-4942-8DE4-469AAA6716DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Játék</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Feb</t>
   </si>
   <si>
-    <t>Márc</t>
-  </si>
-  <si>
     <t>Spotify</t>
   </si>
   <si>
@@ -75,12 +72,26 @@
   </si>
   <si>
     <t>Átlag</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>Apr</t>
+  </si>
+  <si>
+    <t>May</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="168" formatCode="yyyy/\ m/\ d\.;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -116,9 +127,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -400,30 +414,40 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Munka1"/>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="M22" sqref="G13:M22"/>
+    <sheetView tabSelected="1" zoomScale="179" zoomScaleNormal="120" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1"/>
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -436,8 +460,15 @@
       <c r="D2">
         <v>2500</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>1000</v>
+      </c>
+      <c r="F2">
+        <v>200</v>
+      </c>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -450,10 +481,16 @@
       <c r="D3">
         <v>3100</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>4000</v>
+      </c>
+      <c r="F3">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>2000</v>
@@ -464,8 +501,14 @@
       <c r="D4">
         <v>2000</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -478,10 +521,17 @@
       <c r="D5">
         <v>2700</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>3200</v>
+      </c>
+      <c r="F5">
+        <v>4500</v>
+      </c>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>6000</v>
@@ -492,30 +542,57 @@
       <c r="D6">
         <v>3000</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>3000</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <f>SUM(B$2:B$6)</f>
+        <v>14600</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ref="C7:F7" si="0">SUM(C$2:C$6)</f>
+        <v>13100</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>13300</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>11200</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>7900</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excel added to 11, word added to 10, word added to 9, plan finished till march
</commit_message>
<xml_diff>
--- a/docs/projects/excel/01/01.xlsx
+++ b/docs/projects/excel/01/01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\digitalis_kultura\docs\projects\excel\01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E1A7DB-0C06-4BC1-8E76-01987F456B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1528145-24FC-443B-A989-92853803D6AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week01-Ismétlés" sheetId="1" r:id="rId1"/>
@@ -480,14 +480,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1353,6 +1352,375 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="hu-HU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="hu-HU"/>
+              <a:t>Results</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="hu-HU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-E525-4F81-8990-7F0FAB686A46}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Week02 - Decision factors'!$A$4:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Fast food worker</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Football player</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Truck driver</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Programmer</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Engineer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Week02 - Decision factors'!$L$4:$L$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>57</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E525-4F81-8990-7F0FAB686A46}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="1246670720"/>
+        <c:axId val="1246688192"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="1246670720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="hu-HU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1246688192"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1246688192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="hu-HU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1246670720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="hu-HU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1433,6 +1801,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2407,6 +2815,500 @@
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2508,6 +3410,47 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagram 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4613E1F-5C10-347F-FCAB-4FE6D5BD8309}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2975,14 +3918,14 @@
   </sheetPr>
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3.7109375" bestFit="1" customWidth="1"/>
@@ -2993,33 +3936,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="66" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="B2" t="s">
         <v>41</v>
       </c>
       <c r="C2">
@@ -3033,18 +3976,18 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C4">
@@ -3056,15 +3999,15 @@
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="8">
         <f>C4/C$2</f>
         <v>1</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="8">
         <f t="shared" ref="H4:I19" si="0">D4/D$2</f>
         <v>0.93</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="8">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -3074,10 +4017,10 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C5">
@@ -3089,15 +4032,15 @@
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="G5" s="9">
-        <f t="shared" ref="G5:G20" si="1">C5/C$2</f>
+      <c r="G5" s="8">
+        <f t="shared" ref="G5:G18" si="1">C5/C$2</f>
         <v>0.9</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="8">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="8">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -3107,10 +4050,10 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C6">
@@ -3122,15 +4065,15 @@
       <c r="E6">
         <v>1</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="8">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="8">
         <f t="shared" si="0"/>
         <v>0.82</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="8">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -3140,10 +4083,10 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C7">
@@ -3155,15 +4098,15 @@
       <c r="E7">
         <v>1</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="8">
         <f>C7/C$2</f>
         <v>0.9</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="8">
         <f t="shared" si="0"/>
         <v>0.73</v>
       </c>
-      <c r="I7" s="9">
+      <c r="I7" s="8">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -3173,10 +4116,10 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C8">
@@ -3188,15 +4131,15 @@
       <c r="E8">
         <v>1</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="8">
         <f>C8/C$2</f>
         <v>1</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="8">
         <f t="shared" si="0"/>
         <v>0.59</v>
       </c>
-      <c r="I8" s="9">
+      <c r="I8" s="8">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -3206,10 +4149,10 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C9">
@@ -3221,15 +4164,15 @@
       <c r="E9">
         <v>1</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="8">
         <f>C9/C$2</f>
         <v>0.9</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="8">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I9" s="8">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -3239,10 +4182,10 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C10">
@@ -3254,15 +4197,15 @@
       <c r="E10">
         <v>0</v>
       </c>
-      <c r="G10" s="9">
-        <f t="shared" ref="G10:G20" si="3">C10/C$2</f>
+      <c r="G10" s="8">
+        <f t="shared" ref="G10" si="3">C10/C$2</f>
         <v>0.8</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="8">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I10" s="9">
+      <c r="I10" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3272,10 +4215,10 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C11">
@@ -3287,15 +4230,15 @@
       <c r="E11">
         <v>1</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="8">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H11" s="8">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I11" s="9">
+      <c r="I11" s="8">
         <f>E11/E$2</f>
         <v>1</v>
       </c>
@@ -3305,10 +4248,10 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C12">
@@ -3320,15 +4263,15 @@
       <c r="E12">
         <v>1</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="8">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="8">
         <f t="shared" si="0"/>
         <v>0.67</v>
       </c>
-      <c r="I12" s="9">
+      <c r="I12" s="8">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -3338,10 +4281,10 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C13">
@@ -3353,15 +4296,15 @@
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="8">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H13" s="8">
         <f>D13/D$2</f>
         <v>0.7</v>
       </c>
-      <c r="I13" s="9">
+      <c r="I13" s="8">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -3371,10 +4314,10 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>43</v>
       </c>
       <c r="C14">
@@ -3386,15 +4329,15 @@
       <c r="E14">
         <v>1</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="8">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H14" s="8">
         <f>D14/D$2</f>
         <v>0.8</v>
       </c>
-      <c r="I14" s="9">
+      <c r="I14" s="8">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -3404,10 +4347,10 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" t="s">
         <v>44</v>
       </c>
       <c r="C15">
@@ -3419,15 +4362,15 @@
       <c r="E15">
         <v>1</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="8">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="8">
         <f t="shared" si="0"/>
         <v>0.9</v>
       </c>
-      <c r="I15" s="9">
+      <c r="I15" s="8">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -3437,10 +4380,10 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" t="s">
         <v>45</v>
       </c>
       <c r="C16">
@@ -3452,15 +4395,15 @@
       <c r="E16">
         <v>0</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="8">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
-      <c r="H16" s="9">
+      <c r="H16" s="8">
         <f t="shared" si="0"/>
         <v>0.45</v>
       </c>
-      <c r="I16" s="9">
+      <c r="I16" s="8">
         <f>E16/E$2</f>
         <v>0</v>
       </c>
@@ -3470,10 +4413,10 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" t="s">
         <v>46</v>
       </c>
       <c r="C17">
@@ -3485,15 +4428,15 @@
       <c r="E17">
         <v>1</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G17" s="8">
         <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
-      <c r="H17" s="9">
+      <c r="H17" s="8">
         <f>D17/D$2</f>
         <v>0.9</v>
       </c>
-      <c r="I17" s="9">
+      <c r="I17" s="8">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -3503,10 +4446,10 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" t="s">
         <v>47</v>
       </c>
       <c r="C18">
@@ -3518,15 +4461,15 @@
       <c r="E18">
         <v>1</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="8">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="8">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="I18" s="9">
+      <c r="I18" s="8">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -3536,10 +4479,10 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" t="s">
         <v>48</v>
       </c>
       <c r="C19">
@@ -3551,15 +4494,15 @@
       <c r="E19">
         <v>1</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G19" s="8">
         <f>C19/C$2</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="H19" s="9">
+      <c r="H19" s="8">
         <f t="shared" si="0"/>
         <v>0.69</v>
       </c>
-      <c r="I19" s="9">
+      <c r="I19" s="8">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -3569,10 +4512,10 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" t="s">
         <v>55</v>
       </c>
       <c r="C20">
@@ -3584,15 +4527,15 @@
       <c r="E20">
         <v>1</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G20" s="8">
         <f>C20/C$2</f>
         <v>0.6</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20" s="8">
         <f t="shared" ref="H20" si="4">D20/D$2</f>
         <v>0.9</v>
       </c>
-      <c r="I20" s="9">
+      <c r="I20" s="8">
         <f t="shared" ref="I20" si="5">E20/E$2</f>
         <v>1</v>
       </c>
@@ -3602,52 +4545,52 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G22" s="9">
+      <c r="G22" s="8">
         <f>MIN(C4:C20)/10</f>
         <v>0.5</v>
       </c>
-      <c r="H22" s="9">
+      <c r="H22" s="8">
         <f>MIN(D4:D20)/100</f>
         <v>0.45</v>
       </c>
-      <c r="I22" s="9">
+      <c r="I22" s="8">
         <f>MIN(E4:E20)/10</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G23" s="9">
+      <c r="G23" s="8">
         <f>MAX(C4:C20)/10</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="H23" s="9">
+      <c r="H23" s="8">
         <f>MAX(D4:D20)/100</f>
         <v>1</v>
       </c>
-      <c r="I23" s="9">
+      <c r="I23" s="8">
         <f>MAX(E4:E20)/10</f>
         <v>0.1</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="G24" s="9">
+      <c r="G24" s="8">
         <f>AVERAGE(C4:C20)/10</f>
         <v>0.87058823529411755</v>
       </c>
-      <c r="H24" s="9">
+      <c r="H24" s="8">
         <f>AVERAGE(D4:D20)/100</f>
         <v>0.81647058823529406</v>
       </c>
-      <c r="I24" s="9">
+      <c r="I24" s="8">
         <f>AVERAGE(E4:E20)/10</f>
         <v>8.8235294117647051E-2</v>
       </c>
@@ -3703,7 +4646,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3721,259 +4664,259 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="15">
         <v>3</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="16">
         <v>5</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="G3" s="18">
+      <c r="G3" s="17">
         <v>4</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="I3" s="19">
+      <c r="I3" s="18">
         <v>3</v>
       </c>
-      <c r="J3" s="20" t="s">
+      <c r="J3" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="K3" s="20">
+      <c r="K3" s="19">
         <v>1</v>
       </c>
-      <c r="L3" s="21" t="s">
+      <c r="L3" s="20" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="9">
         <v>1</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <f>C$3*B4</f>
         <v>3</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="10">
         <v>5</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="10">
         <f>E$3*D4</f>
         <v>25</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="11">
         <v>1</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="11">
         <f>G$3*F4</f>
         <v>4</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="12">
         <v>4</v>
       </c>
-      <c r="I4" s="13">
+      <c r="I4" s="12">
         <f>I$3*H4</f>
         <v>12</v>
       </c>
-      <c r="J4" s="14">
+      <c r="J4" s="13">
         <v>5</v>
       </c>
-      <c r="K4" s="14">
+      <c r="K4" s="13">
         <f>K$3*J4</f>
         <v>5</v>
       </c>
-      <c r="L4" s="23">
+      <c r="L4" s="22">
         <f>SUM(C4+E4+G4+I4+K4)</f>
         <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <v>5</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="9">
         <f t="shared" ref="C5:E8" si="0">C$3*B5</f>
         <v>15</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="10">
         <v>1</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="10">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="11">
         <v>5</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="11">
         <f t="shared" ref="G5" si="1">G$3*F5</f>
         <v>20</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="12">
         <v>2</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="12">
         <f t="shared" ref="I5:K5" si="2">I$3*H5</f>
         <v>6</v>
       </c>
-      <c r="J5" s="14">
+      <c r="J5" s="13">
         <v>1</v>
       </c>
-      <c r="K5" s="14">
+      <c r="K5" s="13">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="L5" s="23">
+      <c r="L5" s="22">
         <f t="shared" ref="L5:L8" si="3">SUM(C5+E5+G5+I5+K5)</f>
         <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <v>3</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="10">
         <v>4</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="10">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="11">
         <v>3</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="11">
         <f t="shared" ref="G6" si="4">G$3*F6</f>
         <v>12</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="12">
         <v>2</v>
       </c>
-      <c r="I6" s="13">
+      <c r="I6" s="12">
         <f t="shared" ref="I6:K6" si="5">I$3*H6</f>
         <v>6</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="13">
         <v>5</v>
       </c>
-      <c r="K6" s="14">
+      <c r="K6" s="13">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="L6" s="23">
+      <c r="L6" s="22">
         <f t="shared" si="3"/>
         <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="9">
         <v>4</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="9">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="10">
         <v>5</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="10">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="11">
         <v>4</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="11">
         <f t="shared" ref="G7" si="6">G$3*F7</f>
         <v>16</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="12">
         <v>4</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I7" s="12">
         <f t="shared" ref="I7:K7" si="7">I$3*H7</f>
         <v>12</v>
       </c>
-      <c r="J7" s="14">
+      <c r="J7" s="13">
         <v>3</v>
       </c>
-      <c r="K7" s="14">
+      <c r="K7" s="13">
         <f t="shared" si="7"/>
         <v>3</v>
       </c>
-      <c r="L7" s="23">
+      <c r="L7" s="22">
         <f t="shared" si="3"/>
         <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="25">
+      <c r="B8" s="24">
         <v>3</v>
       </c>
-      <c r="C8" s="25">
+      <c r="C8" s="24">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="D8" s="26">
+      <c r="D8" s="25">
         <v>4</v>
       </c>
-      <c r="E8" s="26">
+      <c r="E8" s="25">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="F8" s="27">
+      <c r="F8" s="26">
         <v>4</v>
       </c>
-      <c r="G8" s="27">
+      <c r="G8" s="26">
         <f t="shared" ref="G8" si="8">G$3*F8</f>
         <v>16</v>
       </c>
-      <c r="H8" s="28">
+      <c r="H8" s="27">
         <v>3</v>
       </c>
-      <c r="I8" s="28">
+      <c r="I8" s="27">
         <f t="shared" ref="I8:K8" si="9">I$3*H8</f>
         <v>9</v>
       </c>
-      <c r="J8" s="29">
+      <c r="J8" s="28">
         <v>3</v>
       </c>
-      <c r="K8" s="29">
+      <c r="K8" s="28">
         <f t="shared" si="9"/>
         <v>3</v>
       </c>
-      <c r="L8" s="30">
+      <c r="L8" s="29">
         <f t="shared" si="3"/>
         <v>57</v>
       </c>
@@ -3983,6 +4926,7 @@
     <cfRule type="top10" dxfId="0" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3990,7 +4934,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6A2B947-0D6A-4C81-97A8-91DCFA7B6BFD}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>